<commit_message>
Update Pontos de verificação Connect.xlsx
</commit_message>
<xml_diff>
--- a/Pontos de verificação Connect.xlsx
+++ b/Pontos de verificação Connect.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael_Campos\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael_Campos\Documents\GitHub\ConnectFibra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBDDD90-669D-4EA5-95A5-6AE01579BC54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2216B6E-5CF4-48D8-B5CC-52252F5F7A28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{A8A2084A-6900-4F0E-8F79-BE5AB4B1CC6A}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Açoes a ser tomada</t>
   </si>
@@ -102,13 +102,16 @@
   </si>
   <si>
     <t>Verificar como solucianar a situação de clientes com mais de dois meses de atraso que são cobrados.</t>
+  </si>
+  <si>
+    <t>teste 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +140,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,6 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F050EB28-4A87-4399-9100-1F0B4556B92B}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,9 +534,18 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>